<commit_message>
updated mwb and xlsx files
</commit_message>
<xml_diff>
--- a/Step_2/SampleData.xlsx
+++ b/Step_2/SampleData.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jez-kuh/Desktop/ContEd/OSU/CS340_Spring-25_Databases/Assignments/Project/Step_2_Draft/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grantwu/Documents/school/OSU/SP25/CS340/CS-340_Project/Step_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17E26B8-C51C-3C45-A9EF-16F6C4A99F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B79F135-83D3-6A44-B27C-F3CF6E2D3933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67520" yWindow="-7480" windowWidth="30160" windowHeight="17840" activeTab="4" xr2:uid="{999BF072-19F5-894D-A114-BA5FF22337CA}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16600" activeTab="1" xr2:uid="{999BF072-19F5-894D-A114-BA5FF22337CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Bikes" sheetId="1" r:id="rId1"/>
-    <sheet name="StorePersonnel" sheetId="2" r:id="rId2"/>
-    <sheet name="Customers" sheetId="3" r:id="rId3"/>
-    <sheet name="RepairReports" sheetId="4" r:id="rId4"/>
-    <sheet name="SalesReports" sheetId="5" r:id="rId5"/>
+    <sheet name="Contacts" sheetId="6" r:id="rId2"/>
+    <sheet name="StorePersonnel" sheetId="2" r:id="rId3"/>
+    <sheet name="Customers" sheetId="3" r:id="rId4"/>
+    <sheet name="RepairReports" sheetId="4" r:id="rId5"/>
+    <sheet name="SalesReports" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="92">
   <si>
     <t>bikeID</t>
   </si>
@@ -60,9 +61,6 @@
     <t>dateReceived</t>
   </si>
   <si>
-    <t>isCompleted</t>
-  </si>
-  <si>
     <t>Black</t>
   </si>
   <si>
@@ -120,12 +118,6 @@
     <t>Employee Review</t>
   </si>
   <si>
-    <t>* 0 until reviewed?</t>
-  </si>
-  <si>
-    <t>*is isCompleted redundant information?</t>
-  </si>
-  <si>
     <t>personnelID</t>
   </si>
   <si>
@@ -201,9 +193,6 @@
     <t>tchen@gmail.com</t>
   </si>
   <si>
-    <t>*how to standardize phone numbers?</t>
-  </si>
-  <si>
     <t>customerID</t>
   </si>
   <si>
@@ -313,6 +302,21 @@
   </si>
   <si>
     <t>remmington</t>
+  </si>
+  <si>
+    <t>contactID</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t>453-197-4228</t>
+  </si>
+  <si>
+    <t>j.johnson@yahoo.com</t>
+  </si>
+  <si>
+    <t>receiveNewsletter</t>
   </si>
 </sst>
 </file>
@@ -390,9 +394,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -430,7 +434,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -536,7 +540,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -678,7 +682,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -686,20 +690,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FD1710-FE74-7042-80E8-05DAF6328513}">
-  <dimension ref="A1:H1048575"/>
+  <dimension ref="A1:G1048575"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="16.6640625" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -718,217 +721,167 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F2" s="2">
         <v>45519</v>
       </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F3" s="2">
         <v>45646</v>
       </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" s="2">
         <v>45691</v>
       </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F5" s="2">
         <v>45698</v>
       </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6" s="2">
         <v>45703</v>
       </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F7" s="2">
         <v>45716</v>
       </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C8" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D8" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F8" s="2">
         <v>45717</v>
       </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F9" s="2">
         <v>45738</v>
       </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G20" s="2"/>
     </row>
     <row r="1048575" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F1048575" s="2"/>
@@ -940,166 +893,293 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B18642F1-FD44-D54B-BA3E-038E478D6CB7}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6">
+        <v>4162228888</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8">
+        <v>4953332345</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{0404906A-8A1F-4848-BADB-7CF75800F6CA}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{F0B20577-C8CA-EE42-B068-DF8760E2F521}"/>
+    <hyperlink ref="E5" r:id="rId3" xr:uid="{25DB78AC-FE51-4440-BAC1-66A195F6BA98}"/>
+    <hyperlink ref="E6" r:id="rId4" xr:uid="{D567B7B7-D91E-2449-B4FB-80845BFE4133}"/>
+    <hyperlink ref="E7" r:id="rId5" xr:uid="{BB3AF9B5-EE14-DD40-B882-8C25CF7D7D4C}"/>
+    <hyperlink ref="E8" r:id="rId6" xr:uid="{DF3D87EB-7033-6041-83B6-AC36AC6CC748}"/>
+    <hyperlink ref="E9" r:id="rId7" xr:uid="{23322305-A690-644E-8E0F-7F03C523A89B}"/>
+    <hyperlink ref="E4" r:id="rId8" xr:uid="{732142A1-1340-604F-8D11-5FBA7043BE7D}"/>
+    <hyperlink ref="E10" r:id="rId9" xr:uid="{6FA286E4-6616-1943-8EE3-CDEC0AF57FDF}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{810D034E-59CB-8849-8CFC-2BC5B3F3E63A}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="13.5" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" customWidth="1"/>
-    <col min="5" max="5" width="24.33203125" customWidth="1"/>
-    <col min="6" max="6" width="17.1640625" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>87</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>34</v>
       </c>
-      <c r="C2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>39</v>
+      <c r="B3">
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>43</v>
+      <c r="B4">
+        <v>4</v>
       </c>
       <c r="C4" t="s">
         <v>44</v>
       </c>
-      <c r="D4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>55</v>
+      <c r="B5">
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5">
-        <v>4162228888</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>49</v>
+      <c r="B6">
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D10" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{48BC61A2-4459-4B46-ACF7-2B40D4A7432B}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{80EFD678-EE28-6E47-96CD-65F1D464A5DF}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{224BB2BA-C4AE-E34E-A626-A25AB353BFCF}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{A1022456-03B2-4B42-A746-FCA70909BF6D}"/>
-    <hyperlink ref="E6" r:id="rId5" xr:uid="{ED40D287-CB3D-3D41-BDDA-C532FFDA2D02}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBE080F8-79BE-4D4D-87A2-7FD1A065E297}">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1112,111 +1192,81 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>87</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>32</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D3">
-        <v>4953332345</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>57</v>
-      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>65</v>
-      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C5" t="s">
-        <v>90</v>
-      </c>
-      <c r="D5" t="s">
-        <v>66</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>67</v>
-      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E9" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{6E315F38-C349-E04B-A535-38716076F04F}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{FBFE2A8C-EE95-404F-BAC8-3C56CD3F6EF9}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{6D4C656A-E24A-7343-B813-8744C88BED8F}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{8F88B4B9-C29B-4545-8759-3D89B09B3CDD}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02951FF6-D513-E944-8474-82A667B46CF4}">
   <dimension ref="A1:G9"/>
   <sheetViews>
@@ -1234,22 +1284,22 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1269,7 +1319,7 @@
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -1289,10 +1339,10 @@
         <v>0.5</v>
       </c>
       <c r="F3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="G3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -1309,7 +1359,7 @@
         <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -1329,7 +1379,7 @@
         <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1349,7 +1399,7 @@
         <v>0.5</v>
       </c>
       <c r="F6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1369,7 +1419,7 @@
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1389,7 +1439,7 @@
         <v>0.25</v>
       </c>
       <c r="F8" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -1409,7 +1459,7 @@
         <v>0.25</v>
       </c>
       <c r="F9" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1418,11 +1468,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D8D82E4-7073-DD48-A91A-D1ABA57987C7}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
@@ -1430,19 +1480,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated PDF, added ER diagram, created INSERT statements
</commit_message>
<xml_diff>
--- a/Step_2/SampleData.xlsx
+++ b/Step_2/SampleData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grantwu/Documents/school/OSU/SP25/CS340/CS-340_Project/Step_2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jez-kuh/Desktop/ContEd/OSU/CS340_Spring-25_Databases/CS-340_Project/Step_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B79F135-83D3-6A44-B27C-F3CF6E2D3933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2491AD7-A762-CA41-AF12-D49BD569C12A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16600" activeTab="1" xr2:uid="{999BF072-19F5-894D-A114-BA5FF22337CA}"/>
+    <workbookView xWindow="2660" yWindow="1880" windowWidth="14480" windowHeight="16600" activeTab="4" xr2:uid="{999BF072-19F5-894D-A114-BA5FF22337CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Bikes" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="93">
   <si>
     <t>bikeID</t>
   </si>
@@ -91,9 +91,6 @@
     <t>Felt</t>
   </si>
   <si>
-    <t>Moutain</t>
-  </si>
-  <si>
     <t>Santa Cruz</t>
   </si>
   <si>
@@ -115,9 +112,6 @@
     <t>Sold</t>
   </si>
   <si>
-    <t>Employee Review</t>
-  </si>
-  <si>
     <t>personnelID</t>
   </si>
   <si>
@@ -317,6 +311,15 @@
   </si>
   <si>
     <t>receiveNewsletter</t>
+  </si>
+  <si>
+    <t>In Review</t>
+  </si>
+  <si>
+    <t>Mountain</t>
+  </si>
+  <si>
+    <t>NULL</t>
   </si>
 </sst>
 </file>
@@ -394,9 +397,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -434,7 +437,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -540,7 +543,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -682,7 +685,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -693,7 +696,7 @@
   <dimension ref="A1:G1048575"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="F9" sqref="A1:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -731,13 +734,13 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F2" s="2">
         <v>45519</v>
@@ -754,10 +757,10 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" s="2">
         <v>45646</v>
@@ -774,10 +777,10 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>90</v>
       </c>
       <c r="F4" s="2">
         <v>45691</v>
@@ -788,16 +791,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="2">
         <v>45698</v>
@@ -814,10 +817,10 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6" s="2">
         <v>45703</v>
@@ -834,10 +837,10 @@
         <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F7" s="2">
         <v>45716</v>
@@ -848,16 +851,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" t="s">
         <v>78</v>
       </c>
-      <c r="D8" t="s">
-        <v>80</v>
-      </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F8" s="2">
         <v>45717</v>
@@ -877,7 +880,7 @@
         <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F9" s="2">
         <v>45738</v>
@@ -896,27 +899,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B18642F1-FD44-D54B-BA3E-038E478D6CB7}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -924,16 +927,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
         <v>31</v>
       </c>
-      <c r="C2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -941,16 +944,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" t="s">
         <v>36</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="D3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -958,16 +961,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" t="s">
         <v>58</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="D4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -975,16 +978,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
         <v>40</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="D5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -992,16 +995,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D6">
         <v>4162228888</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1009,16 +1012,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" t="s">
         <v>46</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="D7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1026,16 +1029,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D8">
         <v>4953332345</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1043,16 +1046,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1060,16 +1063,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="D10" t="s">
-        <v>89</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1093,7 +1096,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="C6" sqref="A1:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1104,13 +1107,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1121,7 +1124,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1132,7 +1135,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1143,7 +1146,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1154,7 +1157,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1165,7 +1168,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1179,7 +1182,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="C5" sqref="A1:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1192,13 +1195,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1253,12 +1256,12 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1270,8 +1273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02951FF6-D513-E944-8474-82A667B46CF4}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1284,22 +1287,22 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1319,7 +1322,7 @@
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -1339,10 +1342,10 @@
         <v>0.5</v>
       </c>
       <c r="F3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -1352,6 +1355,9 @@
       <c r="B4">
         <v>5</v>
       </c>
+      <c r="C4" t="s">
+        <v>92</v>
+      </c>
       <c r="D4" s="2">
         <v>45566</v>
       </c>
@@ -1359,7 +1365,7 @@
         <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -1379,7 +1385,7 @@
         <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1399,7 +1405,7 @@
         <v>0.5</v>
       </c>
       <c r="F6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1419,7 +1425,7 @@
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1439,7 +1445,7 @@
         <v>0.25</v>
       </c>
       <c r="F8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -1459,7 +1465,7 @@
         <v>0.25</v>
       </c>
       <c r="F9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1480,19 +1486,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Combined create and insert SQL statements, updated PDF with correct phone datatype
</commit_message>
<xml_diff>
--- a/Step_2/SampleData.xlsx
+++ b/Step_2/SampleData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jez-kuh/Desktop/ContEd/OSU/CS340_Spring-25_Databases/CS-340_Project/Step_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2491AD7-A762-CA41-AF12-D49BD569C12A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58CDE191-4967-A14A-8788-CF49579B8AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2660" yWindow="1880" windowWidth="14480" windowHeight="16600" activeTab="4" xr2:uid="{999BF072-19F5-894D-A114-BA5FF22337CA}"/>
+    <workbookView xWindow="84200" yWindow="-5380" windowWidth="20760" windowHeight="16360" xr2:uid="{999BF072-19F5-894D-A114-BA5FF22337CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Bikes" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="94">
   <si>
     <t>bikeID</t>
   </si>
@@ -320,6 +320,9 @@
   </si>
   <si>
     <t>NULL</t>
+  </si>
+  <si>
+    <t>Enduro</t>
   </si>
 </sst>
 </file>
@@ -695,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FD1710-FE74-7042-80E8-05DAF6328513}">
   <dimension ref="A1:G1048575"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="A1:F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -814,7 +817,7 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>93</v>
       </c>
       <c r="D6" t="s">
         <v>79</v>
@@ -1273,7 +1276,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02951FF6-D513-E944-8474-82A667B46CF4}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>

</xml_diff>